<commit_message>
Figured out how to get mortality plots out, but can't compare axes
</commit_message>
<xml_diff>
--- a/data/hake_intrasp_220713.xlsx
+++ b/data/hake_intrasp_220713.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sowasser/Desktop/Local/hake-CEATTLE/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7071756-4E49-3649-A308-8E68B0808267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9C9358-B750-C44A-9A95-9692C1D3F144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30080" windowHeight="33340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
@@ -1894,7 +1894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -14853,8 +14853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView zoomScale="175" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>